<commit_message>
an_plan.py: AN planning appears to work (both ACP and summary)
</commit_message>
<xml_diff>
--- a/tests/$data_for_test/planning_big.xlsx
+++ b/tests/$data_for_test/planning_big.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\photrix2023\tests\$data_for_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D689FA7F-7C8B-4CB0-8260-59EB0E2B9A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36AFB72-AC54-4757-817A-A24EE4201972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14250" yWindow="1725" windowWidth="13755" windowHeight="16110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28695" yWindow="810" windowWidth="13350" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>CHILL -35</t>
   </si>
@@ -74,9 +74,6 @@
     <t>WAITUNTIL -2</t>
   </si>
   <si>
-    <t>AFINTERVAL 105</t>
-  </si>
-  <si>
     <t>Plan A ; MP 12746, 3229, 3166.</t>
   </si>
   <si>
@@ -86,36 +83,18 @@
     <t>; ~0155 UTC</t>
   </si>
   <si>
-    <t xml:space="preserve">IMAGE MP_3166 BB=420s(1) 04h 24m 52.9516s  +20° 55' 06.970" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMAGE MP_3229 BB=780s(2) 01h 23m 14.2197s  +25° 19' 09.112" </t>
-  </si>
-  <si>
     <t>Plan B ; MP 12746, 3166.</t>
   </si>
   <si>
-    <t>WAITUNTIL 05:35</t>
-  </si>
-  <si>
     <t>QUITAT 07:35</t>
   </si>
   <si>
-    <t xml:space="preserve">IMAGE MP_12746 BB=900s(2) 01h 22m 30.8099s  +14° 29' 40.308" </t>
-  </si>
-  <si>
     <t>Plan C ; MP 3166, 3229, 858 NEW.</t>
   </si>
   <si>
-    <t xml:space="preserve">IMAGE MP_3229 BB=780s(1) 01h 23m 14.2197s  +25° 19' 09.112" </t>
-  </si>
-  <si>
     <t>; ~0815 UTC</t>
   </si>
   <si>
-    <t xml:space="preserve">IMAGE MP_858 BB=720s(2) 08h 09m 48.5774s  +27° 19' 58.464" </t>
-  </si>
-  <si>
     <t>WAITUNTIL 07:35</t>
   </si>
   <si>
@@ -131,25 +110,49 @@
     <t>QUITAT 12:45</t>
   </si>
   <si>
-    <t xml:space="preserve">IMAGE MP_858 BB=720s(100) 08h 09m 48.5774s  +27° 19' 58.464" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMAGE MP_12746 BB=900s(4) 01h 22m 30.8099s  +14° 29' 40.308" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMAGE MP_3229 BB=780s(3) 01h 23m 14.2197s  +25° 19' 09.112" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMAGE MP_3166 BB=420s(2) 04h 24m 52.9516s  +20° 55' 06.970" </t>
-  </si>
-  <si>
     <t>; comment between first WAITUNTIL and first QUITAT.</t>
   </si>
   <si>
     <t>; comment after first MP_3166.</t>
   </si>
   <si>
-    <t xml:space="preserve">COLOR MP_333 </t>
+    <t xml:space="preserve">IMAGE MP_3229 BB=780s(3)  @ 01h 23m 14.2197s  +25° 19' 09.112" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_3166 BB=420s(1) @ 04h 24m 52.9516s  +20° 55' 06.970" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_3229 BB=780s(2) @ 01h 23m 14.2197s  +25° 19' 09.112" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_12746 BB=900s(2) @ 01h 22m 30.8099s  +14° 29' 40.308" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_3166 BB=420s(2) @ 04h 24m 52.9516s  +20° 55' 06.970" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_3229 BB=780s(1) @ 01h 23m 14.2197s  +25° 19' 09.112" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_858 BB=720s(2) @ 08h 09m 48.5774s  +27° 19' 58.464" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_858 BB=720s(100) @ 08h 09m 48.5774s  +27° 19' 58.464" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_12746 BB=900s(4) @ 01h 22m 30.8099s  +14° 29' 40.308" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLOR MP_333 1.4x @ 06h 00m 00.0s  -01° 00' 00.000" </t>
+  </si>
+  <si>
+    <t>AUTOFOCUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE MP_3166 BB=420s(1) R=150s(2) @ 04h 24m 52.9516s  +20° 55' 06.970" </t>
+  </si>
+  <si>
+    <t>WAITUNTIL 05:50</t>
   </si>
 </sst>
 </file>
@@ -1330,11 +1333,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F84"/>
+  <dimension ref="A2:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1368,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1395,311 +1398,316 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="34" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>24</v>
-      </c>
-    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>31</v>
+    <row r="70" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="81" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="36" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
module an_plan: ACP and summary files test OK
</commit_message>
<xml_diff>
--- a/tests/$data_for_test/planning_big.xlsx
+++ b/tests/$data_for_test/planning_big.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\photrix2023\tests\$data_for_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36AFB72-AC54-4757-817A-A24EE4201972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95480769-188E-4CDC-B322-D26F2D0B8DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28695" yWindow="810" windowWidth="13350" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="1575" windowWidth="11700" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1336,7 +1336,7 @@
   <dimension ref="A2:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>

</xml_diff>